<commit_message>
modified GW init file to extend to new scenario 19
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3GroundWaterDataExtractionInitFile_v1.xlsx
+++ b/notebooks/CalSim3GroundWaterDataExtractionInitFile_v1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830B6773-DBB9-4AFE-9530-CBCEA5613DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B4AEF2-17FC-4A33-B5E8-E86457A590BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="-19125" windowWidth="17460" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -180,27 +180,6 @@
     <t>Demands_Deliveries</t>
   </si>
   <si>
-    <t>A18</t>
-  </si>
-  <si>
-    <t>B18</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>G18</t>
-  </si>
-  <si>
-    <t>H18</t>
-  </si>
-  <si>
-    <t>I18</t>
-  </si>
-  <si>
-    <t>J18</t>
-  </si>
-  <si>
     <t>Inflows Extraction Dir</t>
   </si>
   <si>
@@ -250,6 +229,27 @@
   </si>
   <si>
     <t>GroundWaterVars_CS3</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>B19</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>G19</t>
+  </si>
+  <si>
+    <t>H19</t>
+  </si>
+  <si>
+    <t>I19</t>
+  </si>
+  <si>
+    <t>J19</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -662,7 +662,7 @@
         <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -676,35 +676,35 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -718,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -756,7 +756,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -837,26 +837,26 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -864,13 +864,13 @@
         <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>